<commit_message>
Arreglado el logico de ventas
</commit_message>
<xml_diff>
--- a/Documentos/Rubrica1/ModeloLogico/ventas.xlsx
+++ b/Documentos/Rubrica1/ModeloLogico/ventas.xlsx
@@ -1,22 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28705"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ezequiel\Documents\Drive\Proyectos\BDI\BD1Project2019\Documentos\Rubrica1\ModeloLogico\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8F279F91-3343-40F5-A8E3-556548BF522C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20640" windowHeight="11160" tabRatio="647" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="647"/>
   </bookViews>
   <sheets>
     <sheet name="VENTAS" sheetId="31" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -25,15 +22,12 @@
         <xcalcf:feature name="microsoft.com:RD"/>
       </xcalcf:calcFeatures>
     </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="29">
   <si>
     <t>id</t>
   </si>
@@ -50,9 +44,6 @@
     <t>FK1</t>
   </si>
   <si>
-    <t>fecha</t>
-  </si>
-  <si>
     <t>date</t>
   </si>
   <si>
@@ -74,9 +65,6 @@
     <t>nombre</t>
   </si>
   <si>
-    <t>PAÍS</t>
-  </si>
-  <si>
     <t>FACTURA</t>
   </si>
   <si>
@@ -95,13 +83,43 @@
     <t>FK_Pedido</t>
   </si>
   <si>
-    <t>desc</t>
+    <t>pais</t>
+  </si>
+  <si>
+    <t>check('VEN','COL', USA', 'REPDOM')</t>
+  </si>
+  <si>
+    <t>fechaemision</t>
+  </si>
+  <si>
+    <t>numero</t>
+  </si>
+  <si>
+    <t>DETALLE</t>
+  </si>
+  <si>
+    <t>cantidad</t>
+  </si>
+  <si>
+    <t>FK_Pieza</t>
+  </si>
+  <si>
+    <t>FK_Juego</t>
+  </si>
+  <si>
+    <t>PK1</t>
+  </si>
+  <si>
+    <t>FK2</t>
+  </si>
+  <si>
+    <t>descuento</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -141,7 +159,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -177,8 +195,45 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="33">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -212,8 +267,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -236,8 +301,35 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="33">
+  <cellStyles count="43">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
@@ -254,6 +346,11 @@
     <cellStyle name="Hipervínculo" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
@@ -270,6 +367,11 @@
     <cellStyle name="Hipervínculo visitado" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -540,166 +642,193 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" customWidth="1"/>
+    <col min="3" max="3" width="19.5" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:4" ht="17" thickBot="1">
+      <c r="A1" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="13"/>
+    </row>
+    <row r="2" spans="1:4" ht="17" thickBot="1">
+      <c r="A2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="1"/>
-    </row>
-    <row r="2" spans="1:3" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="1:3" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18" thickTop="1" thickBot="1">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:3" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="18" thickTop="1" thickBot="1">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:3" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="6"/>
+    </row>
+    <row r="5" spans="1:4" ht="18" thickTop="1" thickBot="1">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:3" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="6"/>
+    </row>
+    <row r="6" spans="1:4" ht="34" thickTop="1" thickBot="1">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
-      <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="1:3" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="18" thickTop="1" thickBot="1">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="1"/>
-    </row>
-    <row r="8" spans="1:3" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="18" thickTop="1" thickBot="1">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
+    <row r="9" spans="1:4" ht="15" customHeight="1" thickBot="1">
+      <c r="A9" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="13"/>
+    </row>
+    <row r="10" spans="1:4" ht="17" thickBot="1">
+      <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:3" ht="39" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+      <c r="B10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="1"/>
-    </row>
-    <row r="11" spans="1:3" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="18" thickTop="1" thickBot="1">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="1"/>
-    </row>
-    <row r="12" spans="1:3" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+      <c r="C11" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="18" thickTop="1" thickBot="1">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:3" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:4" ht="18" thickTop="1" thickBot="1">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
-      <c r="C13" s="1"/>
-    </row>
-    <row r="14" spans="1:3" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+    </row>
+    <row r="14" spans="1:4" ht="18" thickTop="1" thickBot="1">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
-      <c r="C14" s="1"/>
-    </row>
-    <row r="15" spans="1:3" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="6"/>
+      <c r="D14" s="7"/>
+    </row>
+    <row r="15" spans="1:4" ht="18" thickTop="1" thickBot="1">
       <c r="A15" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="1"/>
-    </row>
-    <row r="16" spans="1:3" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="18" thickTop="1" thickBot="1">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="1:4" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-    </row>
-    <row r="18" spans="1:4" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="18" thickTop="1" thickBot="1">
+      <c r="A17" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+    </row>
+    <row r="18" spans="1:4" ht="18" thickTop="1" thickBot="1">
       <c r="A18" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:4" ht="18" thickTop="1" thickBot="1">
       <c r="A19" s="2" t="s">
         <v>1</v>
       </c>
@@ -713,7 +842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="18" thickTop="1" thickBot="1">
       <c r="A20" s="2" t="s">
         <v>2</v>
       </c>
@@ -721,7 +850,7 @@
       <c r="C20" s="2"/>
       <c r="D20" s="4"/>
     </row>
-    <row r="21" spans="1:4" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="18" thickTop="1" thickBot="1">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -729,48 +858,48 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="18" thickTop="1" thickBot="1">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="4"/>
     </row>
-    <row r="23" spans="1:4" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="18" thickTop="1" thickBot="1">
       <c r="A23" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="18" thickTop="1" thickBot="1">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="1:4" ht="38.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B25" s="7"/>
+    <row r="25" spans="1:4" ht="38.25" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A25" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="9"/>
       <c r="C25" s="1"/>
     </row>
-    <row r="26" spans="1:4" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="18" thickTop="1" thickBot="1">
       <c r="A26" s="5" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="C26" s="1"/>
     </row>
-    <row r="27" spans="1:4" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="18" thickTop="1" thickBot="1">
       <c r="A27" s="3" t="s">
         <v>1</v>
       </c>
@@ -779,99 +908,115 @@
       </c>
       <c r="C27" s="1"/>
     </row>
-    <row r="28" spans="1:4" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="18" thickTop="1" thickBot="1">
       <c r="A28" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B28" s="3"/>
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="1:4" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="18" thickTop="1" thickBot="1">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="1:4" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="18" thickTop="1" thickBot="1">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="1"/>
     </row>
-    <row r="31" spans="1:4" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="18" thickTop="1" thickBot="1">
       <c r="A31" s="3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C31" s="1"/>
     </row>
-    <row r="32" spans="1:4" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" ht="17" thickTop="1">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
     </row>
-    <row r="33" spans="1:3" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B33" s="6"/>
-      <c r="C33" s="1"/>
-    </row>
-    <row r="34" spans="1:3" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C34" s="1"/>
-    </row>
-    <row r="35" spans="1:3" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C35" s="1"/>
-    </row>
-    <row r="36" spans="1:3" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B36" s="2"/>
-      <c r="C36" s="1"/>
-    </row>
-    <row r="37" spans="1:3" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="1"/>
-    </row>
-    <row r="38" spans="1:3" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="1"/>
-    </row>
-    <row r="39" spans="1:3" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="2" t="s">
+    <row r="33" spans="1:3" ht="15" thickBot="1"/>
+    <row r="34" spans="1:3" ht="17" thickBot="1">
+      <c r="A34" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" s="15"/>
+      <c r="C34" s="16"/>
+    </row>
+    <row r="35" spans="1:3" ht="17" thickBot="1">
+      <c r="A35" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="18" thickTop="1" thickBot="1">
+      <c r="A36" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="18" thickTop="1" thickBot="1">
+      <c r="A37" s="7"/>
+      <c r="B37" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="18" thickTop="1" thickBot="1">
+      <c r="A38" s="7"/>
+      <c r="B38" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="18" thickTop="1" thickBot="1">
+      <c r="A39" s="7"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+    </row>
+    <row r="40" spans="1:3" ht="18" thickTop="1" thickBot="1">
+      <c r="A40" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B40" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C39" s="1"/>
-    </row>
-    <row r="40" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="C40" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="17" thickTop="1">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A34:C34"/>
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="A17:D17"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="86" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <pageSetup scale="86" orientation="portrait" horizontalDpi="360" verticalDpi="360"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>